<commit_message>
feat: Update Excel headers to match user template
</commit_message>
<xml_diff>
--- a/public/sample-invoice-template.xlsx
+++ b/public/sample-invoice-template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Invoices" sheetId="1" r:id="rId1"/>
+    <sheet name="Invoice Template" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,33 +405,31 @@
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="30.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="25.83203125" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" customWidth="1"/>
     <col min="18" max="18" width="18.83203125" customWidth="1"/>
-    <col min="19" max="19" width="16.83203125" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" customWidth="1"/>
     <col min="21" max="21" width="20.83203125" customWidth="1"/>
-    <col min="22" max="22" width="20.83203125" customWidth="1"/>
-    <col min="23" max="23" width="14.83203125" customWidth="1"/>
-    <col min="24" max="24" width="30.83203125" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" customWidth="1"/>
+    <col min="23" max="23" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Invoice No</v>
+        <v>Invoice No.</v>
       </c>
       <c r="B1" t="str">
         <v>Invoice Date</v>
@@ -440,70 +438,64 @@
         <v>Global ID</v>
       </c>
       <c r="D1" t="str">
-        <v>First Name</v>
+        <v>Name</v>
       </c>
       <c r="E1" t="str">
-        <v>Last Name</v>
+        <v>State</v>
       </c>
       <c r="F1" t="str">
-        <v>Membership Type</v>
+        <v>Email Id</v>
       </c>
       <c r="G1" t="str">
-        <v>House Account Code</v>
+        <v>Registration</v>
       </c>
       <c r="H1" t="str">
-        <v>Product Code</v>
+        <v>Membership</v>
       </c>
       <c r="I1" t="str">
-        <v>Product Name</v>
+        <v>Month Total</v>
       </c>
       <c r="J1" t="str">
-        <v>Payment Mode</v>
+        <v>CGST 9%</v>
       </c>
       <c r="K1" t="str">
-        <v>Net Amount</v>
+        <v>SGST 9%</v>
       </c>
       <c r="L1" t="str">
-        <v>CGST Rate</v>
+        <v>CGST 18%</v>
       </c>
       <c r="M1" t="str">
-        <v>CGST Amount</v>
+        <v>SGST 18%</v>
       </c>
       <c r="N1" t="str">
-        <v>SGST Rate</v>
+        <v>Total Tax</v>
       </c>
       <c r="O1" t="str">
-        <v>SGST Amount</v>
+        <v>Description</v>
       </c>
       <c r="P1" t="str">
-        <v>Total Tax</v>
+        <v>Membership Start Date</v>
       </c>
       <c r="Q1" t="str">
-        <v>Total Amount</v>
+        <v>Membership End Date</v>
       </c>
       <c r="R1" t="str">
-        <v>Credit Period Start</v>
+        <v>Payment Start Date</v>
       </c>
       <c r="S1" t="str">
-        <v>Credit Period End</v>
+        <v>Payment End Date</v>
       </c>
       <c r="T1" t="str">
-        <v>Due Date</v>
+        <v>Renewal/Quarterly</v>
       </c>
       <c r="U1" t="str">
-        <v>UTR / Transaction Ref</v>
+        <v>Product</v>
       </c>
       <c r="V1" t="str">
-        <v>Payment Received Date</v>
+        <v>Months</v>
       </c>
       <c r="W1" t="str">
-        <v>Payment Status</v>
-      </c>
-      <c r="X1" t="str">
-        <v>Remarks</v>
-      </c>
-      <c r="Y1" t="str">
-        <v>State Code</v>
+        <v>Calculations of Month</v>
       </c>
     </row>
     <row r="2">
@@ -517,70 +509,64 @@
         <v>SH-MUM-001</v>
       </c>
       <c r="D2" t="str">
-        <v>Rahul</v>
+        <v>Rahul Sharma</v>
       </c>
       <c r="E2" t="str">
-        <v>Sharma</v>
+        <v>Maharashtra</v>
       </c>
       <c r="F2" t="str">
+        <v>rahul.sharma@email.com</v>
+      </c>
+      <c r="G2" t="str">
+        <v>REG001</v>
+      </c>
+      <c r="H2" t="str">
         <v>Every House</v>
       </c>
-      <c r="G2" t="str">
-        <v>HAC001</v>
-      </c>
-      <c r="H2" t="str">
-        <v>MEM-EH</v>
-      </c>
-      <c r="I2" t="str">
-        <v>Every House Annual Membership</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Bank Transfer</v>
+      <c r="I2">
+        <v>295000</v>
+      </c>
+      <c r="J2">
+        <v>22500</v>
       </c>
       <c r="K2">
-        <v>250000</v>
+        <v>22500</v>
       </c>
       <c r="L2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>22500</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>9</v>
-      </c>
-      <c r="O2">
-        <v>22500</v>
-      </c>
-      <c r="P2">
         <v>45000</v>
       </c>
-      <c r="Q2">
-        <v>295000</v>
+      <c r="O2" t="str">
+        <v>Annual Membership Fee</v>
+      </c>
+      <c r="P2" t="str">
+        <v>2026-01-15</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>2027-01-14</v>
       </c>
       <c r="R2" t="str">
         <v>2026-01-15</v>
       </c>
       <c r="S2" t="str">
-        <v>2027-01-14</v>
+        <v>2026-02-15</v>
       </c>
       <c r="T2" t="str">
-        <v>2026-02-15</v>
+        <v>Renewal</v>
       </c>
       <c r="U2" t="str">
-        <v>UTR123456789</v>
-      </c>
-      <c r="V2" t="str">
-        <v>2026-01-20</v>
+        <v>Every House Annual</v>
+      </c>
+      <c r="V2">
+        <v>12</v>
       </c>
       <c r="W2" t="str">
-        <v>Paid</v>
-      </c>
-      <c r="X2" t="str">
-        <v>New membership</v>
-      </c>
-      <c r="Y2" t="str">
-        <v>27</v>
+        <v>Jan 2026 - Jan 2027</v>
       </c>
     </row>
     <row r="3">
@@ -594,70 +580,64 @@
         <v>SH-MUM-002</v>
       </c>
       <c r="D3" t="str">
-        <v>Priya</v>
+        <v>Priya Patel</v>
       </c>
       <c r="E3" t="str">
-        <v>Patel</v>
+        <v>Maharashtra</v>
       </c>
       <c r="F3" t="str">
+        <v>priya.patel@email.com</v>
+      </c>
+      <c r="G3" t="str">
+        <v>REG002</v>
+      </c>
+      <c r="H3" t="str">
         <v>Local House</v>
       </c>
-      <c r="G3" t="str">
-        <v>HAC002</v>
-      </c>
-      <c r="H3" t="str">
-        <v>MEM-LH</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Local House Annual Membership</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Credit Card</v>
+      <c r="I3">
+        <v>177000</v>
+      </c>
+      <c r="J3">
+        <v>13500</v>
       </c>
       <c r="K3">
-        <v>150000</v>
+        <v>13500</v>
       </c>
       <c r="L3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>13500</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>9</v>
-      </c>
-      <c r="O3">
-        <v>13500</v>
-      </c>
-      <c r="P3">
         <v>27000</v>
       </c>
-      <c r="Q3">
-        <v>177000</v>
+      <c r="O3" t="str">
+        <v>Annual Membership Fee</v>
+      </c>
+      <c r="P3" t="str">
+        <v>2026-01-16</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>2027-01-15</v>
       </c>
       <c r="R3" t="str">
         <v>2026-01-16</v>
       </c>
       <c r="S3" t="str">
-        <v>2027-01-15</v>
+        <v>2026-02-16</v>
       </c>
       <c r="T3" t="str">
-        <v>2026-02-16</v>
+        <v>New</v>
       </c>
       <c r="U3" t="str">
-        <v/>
-      </c>
-      <c r="V3" t="str">
-        <v/>
+        <v>Local House Annual</v>
+      </c>
+      <c r="V3">
+        <v>12</v>
       </c>
       <c r="W3" t="str">
-        <v>Pending</v>
-      </c>
-      <c r="X3" t="str">
-        <v>Renewal</v>
-      </c>
-      <c r="Y3" t="str">
-        <v>27</v>
+        <v>Jan 2026 - Jan 2027</v>
       </c>
     </row>
     <row r="4">
@@ -671,70 +651,64 @@
         <v>SH-MUM-003</v>
       </c>
       <c r="D4" t="str">
-        <v>Amit</v>
+        <v>Amit Desai</v>
       </c>
       <c r="E4" t="str">
-        <v>Desai</v>
+        <v>Gujarat</v>
       </c>
       <c r="F4" t="str">
+        <v>amit.desai@email.com</v>
+      </c>
+      <c r="G4" t="str">
+        <v>REG003</v>
+      </c>
+      <c r="H4" t="str">
         <v>Under 27</v>
       </c>
-      <c r="G4" t="str">
-        <v>HAC003</v>
-      </c>
-      <c r="H4" t="str">
-        <v>MEM-U27</v>
-      </c>
-      <c r="I4" t="str">
+      <c r="I4">
+        <v>88500</v>
+      </c>
+      <c r="J4">
+        <v>6750</v>
+      </c>
+      <c r="K4">
+        <v>6750</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>13500</v>
+      </c>
+      <c r="O4" t="str">
         <v>Under 27 Membership</v>
       </c>
-      <c r="J4" t="str">
-        <v>UPI</v>
-      </c>
-      <c r="K4">
-        <v>75000</v>
-      </c>
-      <c r="L4">
-        <v>9</v>
-      </c>
-      <c r="M4">
-        <v>6750</v>
-      </c>
-      <c r="N4">
-        <v>9</v>
-      </c>
-      <c r="O4">
-        <v>6750</v>
-      </c>
-      <c r="P4">
-        <v>13500</v>
-      </c>
-      <c r="Q4">
-        <v>88500</v>
+      <c r="P4" t="str">
+        <v>2026-01-17</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>2027-01-16</v>
       </c>
       <c r="R4" t="str">
         <v>2026-01-17</v>
       </c>
       <c r="S4" t="str">
-        <v>2027-01-16</v>
+        <v>2026-02-17</v>
       </c>
       <c r="T4" t="str">
-        <v>2026-02-17</v>
+        <v>New</v>
       </c>
       <c r="U4" t="str">
-        <v>UPI789456123</v>
-      </c>
-      <c r="V4" t="str">
-        <v>2026-01-17</v>
+        <v>Under 27 Annual</v>
+      </c>
+      <c r="V4">
+        <v>12</v>
       </c>
       <c r="W4" t="str">
-        <v>Paid</v>
-      </c>
-      <c r="X4" t="str">
-        <v>New member - Under 27 program</v>
-      </c>
-      <c r="Y4" t="str">
-        <v>27</v>
+        <v>Jan 2026 - Jan 2027</v>
       </c>
     </row>
     <row r="5">
@@ -748,70 +722,64 @@
         <v>SH-MUM-004</v>
       </c>
       <c r="D5" t="str">
-        <v>Sneha</v>
+        <v>Sneha Kapoor</v>
       </c>
       <c r="E5" t="str">
-        <v>Kapoor</v>
+        <v>Maharashtra</v>
       </c>
       <c r="F5" t="str">
+        <v>sneha.kapoor@email.com</v>
+      </c>
+      <c r="G5" t="str">
+        <v>REG004</v>
+      </c>
+      <c r="H5" t="str">
         <v>Every House</v>
       </c>
-      <c r="G5" t="str">
-        <v>HAC004</v>
-      </c>
-      <c r="H5" t="str">
-        <v>MEM-EH-Q</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Every House Quarterly</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Bank Transfer</v>
+      <c r="I5">
+        <v>100300</v>
+      </c>
+      <c r="J5">
+        <v>7650</v>
       </c>
       <c r="K5">
-        <v>85000</v>
+        <v>7650</v>
       </c>
       <c r="L5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>7650</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>9</v>
-      </c>
-      <c r="O5">
-        <v>7650</v>
-      </c>
-      <c r="P5">
         <v>15300</v>
       </c>
-      <c r="Q5">
-        <v>100300</v>
+      <c r="O5" t="str">
+        <v>Quarterly Membership Fee</v>
+      </c>
+      <c r="P5" t="str">
+        <v>2026-01-18</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>2026-04-17</v>
       </c>
       <c r="R5" t="str">
         <v>2026-01-18</v>
       </c>
       <c r="S5" t="str">
-        <v>2026-04-17</v>
+        <v>2026-02-18</v>
       </c>
       <c r="T5" t="str">
-        <v>2026-02-18</v>
+        <v>Quarterly</v>
       </c>
       <c r="U5" t="str">
-        <v/>
-      </c>
-      <c r="V5" t="str">
-        <v/>
+        <v>Every House Quarterly</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
       </c>
       <c r="W5" t="str">
-        <v>Pending</v>
-      </c>
-      <c r="X5" t="str">
-        <v>Quarterly payment plan</v>
-      </c>
-      <c r="Y5" t="str">
-        <v>27</v>
+        <v>Jan 2026 - Apr 2026</v>
       </c>
     </row>
     <row r="6">
@@ -825,75 +793,69 @@
         <v>SH-MUM-005</v>
       </c>
       <c r="D6" t="str">
-        <v>Vikram</v>
+        <v>Vikram Singh</v>
       </c>
       <c r="E6" t="str">
-        <v>Mehta</v>
+        <v>Delhi</v>
       </c>
       <c r="F6" t="str">
+        <v>vikram.singh@corporate.com</v>
+      </c>
+      <c r="G6" t="str">
+        <v>REG005</v>
+      </c>
+      <c r="H6" t="str">
         <v>Corporate</v>
       </c>
-      <c r="G6" t="str">
-        <v>HAC005</v>
-      </c>
-      <c r="H6" t="str">
-        <v>MEM-CORP</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Corporate Membership</v>
-      </c>
-      <c r="J6" t="str">
-        <v>Cheque</v>
+      <c r="I6">
+        <v>500000</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>9</v>
+        <v>45000</v>
       </c>
       <c r="M6">
         <v>45000</v>
       </c>
       <c r="N6">
-        <v>9</v>
-      </c>
-      <c r="O6">
-        <v>45000</v>
-      </c>
-      <c r="P6">
         <v>90000</v>
       </c>
-      <c r="Q6">
-        <v>590000</v>
+      <c r="O6" t="str">
+        <v>Corporate Membership (5 users)</v>
+      </c>
+      <c r="P6" t="str">
+        <v>2026-01-19</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>2027-01-18</v>
       </c>
       <c r="R6" t="str">
         <v>2026-01-19</v>
       </c>
       <c r="S6" t="str">
-        <v>2027-01-18</v>
+        <v>2026-02-19</v>
       </c>
       <c r="T6" t="str">
-        <v>2026-02-19</v>
+        <v>Renewal</v>
       </c>
       <c r="U6" t="str">
-        <v>CHQ456789</v>
-      </c>
-      <c r="V6" t="str">
-        <v>2026-01-25</v>
+        <v>Corporate Annual</v>
+      </c>
+      <c r="V6">
+        <v>12</v>
       </c>
       <c r="W6" t="str">
-        <v>Paid</v>
-      </c>
-      <c r="X6" t="str">
-        <v>Corporate account - 5 memberships</v>
-      </c>
-      <c r="Y6" t="str">
-        <v>27</v>
+        <v>Jan 2026 - Jan 2027</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Y6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:W6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>